<commit_message>
Update the bar charts
modified:   cpu_network_performance.xlsx
</commit_message>
<xml_diff>
--- a/data/cpu_network_performance.xlsx
+++ b/data/cpu_network_performance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Documents/pci-passthrough/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Documents/pci-passthrough/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26100" windowHeight="14800" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26100" windowHeight="14800" tabRatio="993" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
@@ -316,6 +316,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -641,11 +642,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-324466736"/>
-        <c:axId val="-347665152"/>
+        <c:axId val="-320773392"/>
+        <c:axId val="-320771072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-324466736"/>
+        <c:axId val="-320773392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +689,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347665152"/>
+        <c:crossAx val="-320771072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -696,7 +697,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-347665152"/>
+        <c:axId val="-320771072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-324466736"/>
+        <c:crossAx val="-320773392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -761,6 +762,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -872,6 +874,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1197,11 +1200,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-348095776"/>
-        <c:axId val="-454517408"/>
+        <c:axId val="-320829472"/>
+        <c:axId val="-324725440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-348095776"/>
+        <c:axId val="-320829472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,7 +1247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-454517408"/>
+        <c:crossAx val="-324725440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1252,9 +1255,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-454517408"/>
+        <c:axId val="-324725440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1303,7 +1307,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-348095776"/>
+        <c:crossAx val="-320829472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1317,6 +1321,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2489,7 +2494,7 @@
         <xdr:cNvPr id="3" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2532,7 +2537,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2854,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
@@ -3306,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4195,8 +4200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Upload performance results from the experiment 132 to 151
</commit_message>
<xml_diff>
--- a/data/cpu_network_performance.xlsx
+++ b/data/cpu_network_performance.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18828"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binghamton0-my.sharepoint.com/personal/tcheng8_binghamton_edu/Documents/itri/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="153" documentId="29D64C58418C33B10946EF46E32E0DF452F98909" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{802C109F-8405-4982-A8CA-2DB5EB8FB8A7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10350" windowHeight="6555" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="1820" yWindow="460" windowWidth="25960" windowHeight="14700" tabRatio="993" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
     <sheet name="atop_1p26_2010" sheetId="4" r:id="rId2"/>
     <sheet name="atop_2p3p0_2017" sheetId="6" r:id="rId3"/>
+    <sheet name="poll_halt_ns" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="171026" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="86">
   <si>
     <t>experiment</t>
   </si>
@@ -181,6 +183,27 @@
     <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0</t>
   </si>
   <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, no kvm modules, idle=hlt</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, no kvm modules, idle=poll</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, no kvm modules, idle=hlt, max performance</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, no kvm modules, idle=poll, max performance</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, max performance, halt_poll_ns=400000</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, max performance, halt_poll_ns=0</t>
+  </si>
+  <si>
+    <t>1 pCPU, 3GB RAM, 1 pNIC, atop 2.3.0, max performance, halt_poll_ns=200000</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -257,13 +280,25 @@
   </si>
   <si>
     <t>process account error?</t>
+  </si>
+  <si>
+    <t>baremetal</t>
+  </si>
+  <si>
+    <t>halt_poll_ns=400000</t>
+  </si>
+  <si>
+    <t>halt_poll_ns=0</t>
+  </si>
+  <si>
+    <t>halt_poll_ns=200000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -331,7 +366,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -361,12 +396,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,7 +460,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -748,11 +785,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-347616528"/>
-        <c:axId val="-347791216"/>
+        <c:axId val="-140991760"/>
+        <c:axId val="-140989440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-347616528"/>
+        <c:axId val="-140991760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,7 +832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347791216"/>
+        <c:crossAx val="-140989440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -803,7 +840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-347791216"/>
+        <c:axId val="-140989440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347616528"/>
+        <c:crossAx val="-140991760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -868,7 +905,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -980,7 +1016,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1306,11 +1341,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-347917584"/>
-        <c:axId val="-347201872"/>
+        <c:axId val="-140945472"/>
+        <c:axId val="-140942720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-347917584"/>
+        <c:axId val="-140945472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1388,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347201872"/>
+        <c:crossAx val="-140942720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1361,7 +1396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-347201872"/>
+        <c:axId val="-140942720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1413,7 +1448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-347917584"/>
+        <c:crossAx val="-140945472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1427,7 +1462,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2635,7 +2669,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>40005</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2962,23 +2996,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView topLeftCell="A111" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="102.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2995,7 +3029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>25</v>
       </c>
@@ -3012,7 +3046,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>26</v>
       </c>
@@ -3029,7 +3063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>27</v>
       </c>
@@ -3046,7 +3080,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>28</v>
       </c>
@@ -3063,7 +3097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>29</v>
       </c>
@@ -3080,7 +3114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>30</v>
       </c>
@@ -3097,7 +3131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>31</v>
       </c>
@@ -3114,7 +3148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>32</v>
       </c>
@@ -3131,7 +3165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>33</v>
       </c>
@@ -3148,7 +3182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>34</v>
       </c>
@@ -3165,7 +3199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>35</v>
       </c>
@@ -3182,7 +3216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>36</v>
       </c>
@@ -3199,7 +3233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>37</v>
       </c>
@@ -3216,7 +3250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>38</v>
       </c>
@@ -3233,7 +3267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>39</v>
       </c>
@@ -3250,7 +3284,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>40</v>
       </c>
@@ -3267,7 +3301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>41</v>
       </c>
@@ -3284,7 +3318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>42</v>
       </c>
@@ -3301,7 +3335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>43</v>
       </c>
@@ -3318,7 +3352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>44</v>
       </c>
@@ -3335,7 +3369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>45</v>
       </c>
@@ -3352,7 +3386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>46</v>
       </c>
@@ -3369,7 +3403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>47</v>
       </c>
@@ -3386,7 +3420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>48</v>
       </c>
@@ -3403,7 +3437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>49</v>
       </c>
@@ -3420,7 +3454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>50</v>
       </c>
@@ -3437,7 +3471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>51</v>
       </c>
@@ -3454,7 +3488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>52</v>
       </c>
@@ -3471,7 +3505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>53</v>
       </c>
@@ -3488,7 +3522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>54</v>
       </c>
@@ -3505,7 +3539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>55</v>
       </c>
@@ -3522,7 +3556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>56</v>
       </c>
@@ -3539,7 +3573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>57</v>
       </c>
@@ -3556,7 +3590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>58</v>
       </c>
@@ -3573,7 +3607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>59</v>
       </c>
@@ -3590,7 +3624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>60</v>
       </c>
@@ -3607,7 +3641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>61</v>
       </c>
@@ -3624,7 +3658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>62</v>
       </c>
@@ -3641,7 +3675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>63</v>
       </c>
@@ -3658,7 +3692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>64</v>
       </c>
@@ -3675,7 +3709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>65</v>
       </c>
@@ -3692,7 +3726,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>66</v>
       </c>
@@ -3709,7 +3743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>67</v>
       </c>
@@ -3726,7 +3760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>68</v>
       </c>
@@ -3743,7 +3777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>69</v>
       </c>
@@ -3760,7 +3794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>70</v>
       </c>
@@ -3777,7 +3811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>71</v>
       </c>
@@ -3794,7 +3828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>72</v>
       </c>
@@ -3811,7 +3845,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>73</v>
       </c>
@@ -3828,7 +3862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>74</v>
       </c>
@@ -3845,7 +3879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>75</v>
       </c>
@@ -3862,7 +3896,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>76</v>
       </c>
@@ -3879,7 +3913,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>77</v>
       </c>
@@ -3896,7 +3930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>78</v>
       </c>
@@ -3913,7 +3947,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>79</v>
       </c>
@@ -3930,7 +3964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="2">
         <v>80</v>
       </c>
@@ -3947,7 +3981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>81</v>
       </c>
@@ -3964,7 +3998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>82</v>
       </c>
@@ -3981,7 +4015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>83</v>
       </c>
@@ -3998,7 +4032,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>84</v>
       </c>
@@ -4015,7 +4049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>85</v>
       </c>
@@ -4032,7 +4066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>86</v>
       </c>
@@ -4049,7 +4083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>87</v>
       </c>
@@ -4066,7 +4100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>88</v>
       </c>
@@ -4083,7 +4117,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>89</v>
       </c>
@@ -4100,7 +4134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>90</v>
       </c>
@@ -4117,7 +4151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>91</v>
       </c>
@@ -4134,7 +4168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>92</v>
       </c>
@@ -4151,7 +4185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>93</v>
       </c>
@@ -4168,7 +4202,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>94</v>
       </c>
@@ -4185,7 +4219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>95</v>
       </c>
@@ -4202,7 +4236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>96</v>
       </c>
@@ -4219,7 +4253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>97</v>
       </c>
@@ -4236,7 +4270,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>98</v>
       </c>
@@ -4253,7 +4287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>99</v>
       </c>
@@ -4270,7 +4304,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>100</v>
       </c>
@@ -4287,7 +4321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>101</v>
       </c>
@@ -4304,7 +4338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>102</v>
       </c>
@@ -4321,7 +4355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>103</v>
       </c>
@@ -4338,7 +4372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>104</v>
       </c>
@@ -4355,7 +4389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>105</v>
       </c>
@@ -4372,7 +4406,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>106</v>
       </c>
@@ -4389,7 +4423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>107</v>
       </c>
@@ -4406,7 +4440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>108</v>
       </c>
@@ -4423,7 +4457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>109</v>
       </c>
@@ -4440,7 +4474,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>110</v>
       </c>
@@ -4457,7 +4491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>111</v>
       </c>
@@ -4474,7 +4508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>112</v>
       </c>
@@ -4491,7 +4525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>113</v>
       </c>
@@ -4508,7 +4542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>114</v>
       </c>
@@ -4525,7 +4559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>115</v>
       </c>
@@ -4542,7 +4576,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>116</v>
       </c>
@@ -4559,7 +4593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>117</v>
       </c>
@@ -4576,7 +4610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>118</v>
       </c>
@@ -4593,7 +4627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>119</v>
       </c>
@@ -4610,7 +4644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>120</v>
       </c>
@@ -4627,7 +4661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>121</v>
       </c>
@@ -4644,7 +4678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>122</v>
       </c>
@@ -4661,7 +4695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>123</v>
       </c>
@@ -4678,7 +4712,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>124</v>
       </c>
@@ -4695,7 +4729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>125</v>
       </c>
@@ -4712,7 +4746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>126</v>
       </c>
@@ -4729,7 +4763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>127</v>
       </c>
@@ -4746,7 +4780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>128</v>
       </c>
@@ -4763,7 +4797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>129</v>
       </c>
@@ -4777,6 +4811,380 @@
         <v>47</v>
       </c>
       <c r="E110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112">
+        <v>130</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>49</v>
+      </c>
+      <c r="D112" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113">
+        <v>131</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>50</v>
+      </c>
+      <c r="D113" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115">
+        <v>132</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>51</v>
+      </c>
+      <c r="D115" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116">
+        <v>133</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>52</v>
+      </c>
+      <c r="D116" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118">
+        <v>134</v>
+      </c>
+      <c r="B118" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" t="s">
+        <v>53</v>
+      </c>
+      <c r="D118" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119">
+        <v>135</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" t="s">
+        <v>43</v>
+      </c>
+      <c r="E119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120">
+        <v>136</v>
+      </c>
+      <c r="B120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" t="s">
+        <v>53</v>
+      </c>
+      <c r="D120" t="s">
+        <v>44</v>
+      </c>
+      <c r="E120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121">
+        <v>137</v>
+      </c>
+      <c r="B121" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" t="s">
+        <v>53</v>
+      </c>
+      <c r="D121" t="s">
+        <v>45</v>
+      </c>
+      <c r="E121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122">
+        <v>138</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" t="s">
+        <v>53</v>
+      </c>
+      <c r="D122" t="s">
+        <v>46</v>
+      </c>
+      <c r="E122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123">
+        <v>139</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" t="s">
+        <v>53</v>
+      </c>
+      <c r="D123" t="s">
+        <v>47</v>
+      </c>
+      <c r="E123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125">
+        <v>140</v>
+      </c>
+      <c r="B125" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" t="s">
+        <v>54</v>
+      </c>
+      <c r="D125" t="s">
+        <v>42</v>
+      </c>
+      <c r="E125" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126">
+        <v>141</v>
+      </c>
+      <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" t="s">
+        <v>54</v>
+      </c>
+      <c r="D126" t="s">
+        <v>43</v>
+      </c>
+      <c r="E126" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127">
+        <v>142</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+      <c r="D127" t="s">
+        <v>44</v>
+      </c>
+      <c r="E127" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128">
+        <v>143</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+      <c r="D128" t="s">
+        <v>45</v>
+      </c>
+      <c r="E128" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129">
+        <v>144</v>
+      </c>
+      <c r="B129" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129" t="s">
+        <v>54</v>
+      </c>
+      <c r="D129" t="s">
+        <v>46</v>
+      </c>
+      <c r="E129" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130">
+        <v>145</v>
+      </c>
+      <c r="B130" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" t="s">
+        <v>54</v>
+      </c>
+      <c r="D130" t="s">
+        <v>47</v>
+      </c>
+      <c r="E130" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132">
+        <v>146</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" t="s">
+        <v>55</v>
+      </c>
+      <c r="D132" t="s">
+        <v>42</v>
+      </c>
+      <c r="E132" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133">
+        <v>147</v>
+      </c>
+      <c r="B133" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" t="s">
+        <v>55</v>
+      </c>
+      <c r="D133" t="s">
+        <v>43</v>
+      </c>
+      <c r="E133" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134">
+        <v>148</v>
+      </c>
+      <c r="B134" t="s">
+        <v>9</v>
+      </c>
+      <c r="C134" t="s">
+        <v>55</v>
+      </c>
+      <c r="D134" t="s">
+        <v>44</v>
+      </c>
+      <c r="E134" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135">
+        <v>149</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" t="s">
+        <v>55</v>
+      </c>
+      <c r="D135" t="s">
+        <v>45</v>
+      </c>
+      <c r="E135" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136">
+        <v>150</v>
+      </c>
+      <c r="B136" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" t="s">
+        <v>55</v>
+      </c>
+      <c r="D136" t="s">
+        <v>46</v>
+      </c>
+      <c r="E136" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137">
+        <v>151</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" t="s">
+        <v>55</v>
+      </c>
+      <c r="D137" t="s">
+        <v>47</v>
+      </c>
+      <c r="E137" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4791,14 +5199,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.625" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="23.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
@@ -4816,40 +5224,40 @@
     <col min="18" max="16384" width="17.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H1"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1"/>
       <c r="L1" s="15" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
       <c r="O1" s="14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="P1" s="14"/>
       <c r="Q1" s="14"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B2" s="11">
         <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3">
         <v>942</v>
@@ -4859,31 +5267,31 @@
       <c r="J2" s="2"/>
       <c r="K2"/>
       <c r="L2" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="16"/>
       <c r="B3" s="11">
         <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>941</v>
@@ -4891,7 +5299,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="L3" s="5">
         <v>8.3140499999999999</v>
@@ -4912,13 +5320,13 @@
         <v>49.5124</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="16"/>
       <c r="B4" s="11">
         <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3">
         <v>941</v>
@@ -4927,7 +5335,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="L4" s="7">
         <v>15.31</v>
@@ -4948,15 +5356,15 @@
         <v>49.52</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B5" s="11">
         <v>106</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3">
         <v>942</v>
@@ -4965,7 +5373,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L5" s="7">
         <v>63.35</v>
@@ -4986,59 +5394,59 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="13"/>
       <c r="B6" s="11">
         <v>108</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>942</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="13"/>
       <c r="B7" s="11">
         <v>110</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3">
         <v>941</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="B10" s="11">
         <v>100</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D10" s="5">
         <v>8.3140499999999999</v>
@@ -5053,13 +5461,13 @@
         <v>78.652900000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="16"/>
       <c r="B11" s="11">
         <v>102</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D11" s="5">
         <v>5.6198300000000003</v>
@@ -5074,13 +5482,13 @@
         <v>93.495859999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="16"/>
       <c r="B12" s="11">
         <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D12" s="5">
         <v>4.9917400000000001</v>
@@ -5095,15 +5503,15 @@
         <v>94.371859999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B13" s="11">
         <v>106</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5">
         <v>43.008299999999998</v>
@@ -5118,13 +5526,13 @@
         <v>56.991700000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="13"/>
       <c r="B14" s="11">
         <v>108</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5">
         <v>46.966900000000003</v>
@@ -5139,13 +5547,13 @@
         <v>53.190109999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="13"/>
       <c r="B15" s="11">
         <v>110</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D15" s="5">
         <v>49.5124</v>
@@ -5160,52 +5568,52 @@
         <v>50.562019999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="B22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="I22" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B23" s="3">
         <v>0.04</v>
@@ -5217,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="G23" s="8">
         <f t="shared" ref="G23:I30" si="0">B23*$G$31/100</f>
@@ -5232,9 +5640,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B24" s="3">
         <v>0.59</v>
@@ -5246,7 +5654,7 @@
         <v>0.02</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
@@ -5261,9 +5669,9 @@
         <v>216.56600000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B25" s="3">
         <v>8.43</v>
@@ -5275,7 +5683,7 @@
         <v>2.38</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G25" s="8">
         <f t="shared" si="0"/>
@@ -5290,9 +5698,9 @@
         <v>25771.353999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B26" s="3">
         <v>59.73</v>
@@ -5304,7 +5712,7 @@
         <v>93.91</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G26" s="8">
         <f t="shared" si="0"/>
@@ -5319,9 +5727,9 @@
         <v>1016885.6529999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B27" s="3">
         <v>25.72</v>
@@ -5333,7 +5741,7 @@
         <v>0.17</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G27" s="8">
         <f t="shared" si="0"/>
@@ -5348,9 +5756,9 @@
         <v>1840.8110000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B28" s="3">
         <v>5.31</v>
@@ -5362,7 +5770,7 @@
         <v>3.66</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G28" s="8">
         <f t="shared" si="0"/>
@@ -5377,9 +5785,9 @@
         <v>39631.578000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3">
         <v>0.03</v>
@@ -5391,7 +5799,7 @@
         <v>0.02</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G29" s="8">
         <f t="shared" si="0"/>
@@ -5406,9 +5814,9 @@
         <v>216.56600000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B30" s="3">
         <v>0.27</v>
@@ -5420,7 +5828,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
@@ -5435,9 +5843,9 @@
         <v>757.98100000000011</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="F31" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G31" s="3">
         <v>1082830</v>
@@ -5449,37 +5857,37 @@
         <v>1416721</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="B34" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B35" s="3">
         <v>0.15</v>
@@ -5491,7 +5899,7 @@
         <v>0.04</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G35" s="9">
         <f t="shared" ref="G35:I40" si="1">B35*$G$41/100</f>
@@ -5506,9 +5914,9 @@
         <v>1900.164</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B36" s="3">
         <v>22.43</v>
@@ -5520,7 +5928,7 @@
         <v>94.97</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="1"/>
@@ -5535,9 +5943,9 @@
         <v>4511464.3770000003</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B37" s="3">
         <v>5.03</v>
@@ -5549,7 +5957,7 @@
         <v>0.1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G37" s="9">
         <f t="shared" si="1"/>
@@ -5564,9 +5972,9 @@
         <v>4750.41</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B38" s="3">
         <v>1.1000000000000001</v>
@@ -5578,7 +5986,7 @@
         <v>3.37</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G38" s="9">
         <f t="shared" si="1"/>
@@ -5593,9 +6001,9 @@
         <v>160088.81700000001</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B39" s="3">
         <v>71.31</v>
@@ -5607,7 +6015,7 @@
         <v>0.86</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G39" s="9">
         <f t="shared" si="1"/>
@@ -5622,9 +6030,9 @@
         <v>40853.525999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B40" s="3">
         <v>0.24</v>
@@ -5636,7 +6044,7 @@
         <v>0.84</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="1"/>
@@ -5651,9 +6059,9 @@
         <v>39903.443999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="F41" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G41" s="3">
         <v>4750410</v>
@@ -5680,14 +6088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
@@ -5696,92 +6104,91 @@
     <col min="5" max="5" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G1" s="3"/>
       <c r="L1" s="15" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
       <c r="O1" s="14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="P1" s="14"/>
       <c r="Q1" s="14"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="16" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B2" s="11">
         <v>112</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3">
         <v>942</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G2" s="3"/>
       <c r="L2" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="16"/>
       <c r="B3" s="11">
         <v>114</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>942</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="L3" s="5">
         <v>7.7107400000000004</v>
@@ -5802,13 +6209,13 @@
         <v>98.289299999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="16"/>
       <c r="B4" s="11">
         <v>116</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3">
         <v>941</v>
@@ -5817,7 +6224,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="K4" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="L4" s="5">
         <v>14.504099999999999</v>
@@ -5838,15 +6245,15 @@
         <v>98.396699999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B5" s="11">
         <v>118</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3">
         <v>941</v>
@@ -5855,7 +6262,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="K5" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L5" s="5">
         <v>79.578500000000005</v>
@@ -5876,13 +6283,13 @@
         <v>1.60331</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="13"/>
       <c r="B6" s="11">
         <v>120</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>942</v>
@@ -5891,13 +6298,13 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="13"/>
       <c r="B7" s="11">
         <v>122</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3">
         <v>941</v>
@@ -5906,7 +6313,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5915,36 +6322,36 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="B10" s="11">
         <v>112</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D10" s="5">
         <v>9.7520699999999998</v>
@@ -5959,16 +6366,16 @@
         <v>43.033099999999997</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="16"/>
       <c r="B11" s="11">
         <v>114</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D11" s="5">
         <v>5.9338800000000003</v>
@@ -5983,13 +6390,13 @@
         <v>98.471080000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="16"/>
       <c r="B12" s="11">
         <v>116</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D12" s="5">
         <v>5.1074400000000004</v>
@@ -6004,15 +6411,15 @@
         <v>99.074349999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B13" s="11">
         <v>118</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5">
         <v>73.925600000000003</v>
@@ -6027,13 +6434,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="13"/>
       <c r="B14" s="11">
         <v>120</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5">
         <v>88.008300000000006</v>
@@ -6048,13 +6455,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="13"/>
       <c r="B15" s="11">
         <v>122</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D15" s="5">
         <v>98.578500000000005</v>
@@ -6069,7 +6476,7 @@
         <v>99.999989999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6078,665 +6485,1554 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="11">
-        <v>124</v>
+      <c r="B18" s="3">
+        <v>130</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5">
-        <v>7.7107400000000004</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5">
-        <v>14.504099999999999</v>
+        <v>0.10743800000000001</v>
       </c>
       <c r="F18" s="5">
-        <v>79.578500000000005</v>
+        <v>2.91736</v>
       </c>
       <c r="G18" s="5">
-        <v>94.082599999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.0247980000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="16"/>
       <c r="B19" s="11">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D19" s="5">
-        <v>6.5371899999999998</v>
+        <v>7.7107400000000004</v>
       </c>
       <c r="E19" s="5">
-        <v>6.5537200000000002</v>
+        <v>14.504099999999999</v>
       </c>
       <c r="F19" s="5">
-        <v>92</v>
+        <v>79.578500000000005</v>
       </c>
       <c r="G19" s="5">
-        <v>98.553719999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94.082599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="16"/>
       <c r="B20" s="11">
+        <v>125</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5">
+        <v>6.5371899999999998</v>
+      </c>
+      <c r="E20" s="5">
+        <v>6.5537200000000002</v>
+      </c>
+      <c r="F20" s="5">
+        <v>92</v>
+      </c>
+      <c r="G20" s="5">
+        <v>98.553719999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="16"/>
+      <c r="B21" s="11">
         <v>126</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="5">
         <v>5.0330599999999999</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E21" s="5">
         <v>5.0495900000000002</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F21" s="5">
         <v>94.033100000000005</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G21" s="5">
         <v>99.082689999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="11">
-        <v>127</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="5">
-        <v>74.834699999999998</v>
-      </c>
-      <c r="E21" s="5">
-        <v>81.611599999999996</v>
-      </c>
-      <c r="F21" s="5">
-        <v>18.388400000000001</v>
-      </c>
-      <c r="G21" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:9">
+      <c r="A22" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="B22" s="11">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="5">
-        <v>87.504099999999994</v>
-      </c>
-      <c r="E22" s="5">
-        <v>87.5124</v>
-      </c>
-      <c r="F22" s="5">
-        <v>12.4876</v>
-      </c>
-      <c r="G22" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4.1322299999999999E-2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1.2727299999999999</v>
+      </c>
+      <c r="G22" s="7">
+        <v>1.3140523</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="13"/>
       <c r="B23" s="11">
+        <v>127</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5">
+        <v>74.834699999999998</v>
+      </c>
+      <c r="E23" s="5">
+        <v>81.611599999999996</v>
+      </c>
+      <c r="F23" s="5">
+        <v>18.388400000000001</v>
+      </c>
+      <c r="G23" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="13"/>
+      <c r="B24" s="11">
+        <v>128</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="5">
+        <v>87.504099999999994</v>
+      </c>
+      <c r="E24" s="5">
+        <v>87.5124</v>
+      </c>
+      <c r="F24" s="5">
+        <v>12.4876</v>
+      </c>
+      <c r="G24" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="13"/>
+      <c r="B25" s="11">
         <v>129</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="5">
+      <c r="C25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5">
         <v>98.289299999999997</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E25" s="5">
         <v>98.396699999999996</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F25" s="5">
         <v>1.60331</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G25" s="5">
         <v>100.00001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="3"/>
+    <row r="26" spans="1:9">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="F26" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="F28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30">
         <v>0.24</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>0.47</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>0.02</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="8">
-        <f>B28*$G$35/100</f>
+      <c r="F30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="8">
+        <f>B30*$G$37/100</f>
         <v>2582.0831999999996</v>
       </c>
-      <c r="H28" s="8">
-        <f t="shared" ref="H28:I34" si="0">C28*$G$35/100</f>
+      <c r="H30" s="8">
+        <f t="shared" ref="H30:I36" si="0">C30*$G$37/100</f>
         <v>5056.5796</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I30" s="8">
         <f t="shared" si="0"/>
         <v>215.17359999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29">
+    <row r="31" spans="1:9">
+      <c r="A31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31">
         <v>7.53</v>
       </c>
-      <c r="C29">
+      <c r="C31">
         <v>7.64</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>3.08</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="8">
-        <f t="shared" ref="G29:G34" si="1">B29*$G$35/100</f>
+      <c r="F31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" ref="G31:G36" si="1">B31*$G$37/100</f>
         <v>81012.860400000005</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H31" s="8">
         <f t="shared" si="0"/>
         <v>82196.315199999997</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I31" s="8">
         <f t="shared" si="0"/>
         <v>33136.734400000001</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30">
+    <row r="32" spans="1:9">
+      <c r="A32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32">
         <v>59.39</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>59.35</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <v>92.84</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="8">
+      <c r="F32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="8">
         <f t="shared" si="1"/>
         <v>638958.00520000001</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H32" s="8">
         <f t="shared" si="0"/>
         <v>638527.65800000005</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I32" s="8">
         <f t="shared" si="0"/>
         <v>998835.85120000003</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31">
+    <row r="33" spans="1:9">
+      <c r="A33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33">
         <v>27.21</v>
       </c>
-      <c r="C31">
+      <c r="C33">
         <v>26.94</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>0.16</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="8">
+      <c r="F33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="8">
         <f t="shared" si="1"/>
         <v>292743.68280000001</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H33" s="8">
         <f t="shared" si="0"/>
         <v>289838.83920000005</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I33" s="8">
         <f t="shared" si="0"/>
         <v>1721.3887999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32">
+    <row r="34" spans="1:9">
+      <c r="A34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34">
         <v>5.54</v>
       </c>
-      <c r="C32">
+      <c r="C34">
         <v>5.41</v>
       </c>
-      <c r="D32">
+      <c r="D34">
         <v>4.09</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G32" s="8">
+      <c r="F34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="8">
         <f t="shared" si="1"/>
         <v>59603.087199999994</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H34" s="8">
         <f t="shared" si="0"/>
         <v>58204.4588</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I34" s="8">
         <f t="shared" si="0"/>
         <v>44003.001199999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33">
+    <row r="35" spans="1:9">
+      <c r="A35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35">
         <v>0.02</v>
       </c>
-      <c r="C33">
+      <c r="C35">
         <v>0.04</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>0.02</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="8">
+      <c r="F35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="8">
         <f t="shared" si="1"/>
         <v>215.17359999999999</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H35" s="8">
         <f t="shared" si="0"/>
         <v>430.34719999999999</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I35" s="8">
         <f t="shared" si="0"/>
         <v>215.17359999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34">
+    <row r="36" spans="1:9">
+      <c r="A36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36">
         <v>0.21</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>0.18</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="8">
+      <c r="F36" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="8">
         <f t="shared" si="1"/>
         <v>2259.3227999999999</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H36" s="8">
         <f t="shared" si="0"/>
         <v>1936.5623999999998</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I36" s="8">
         <f t="shared" si="0"/>
         <v>753.10760000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
+    <row r="37" spans="1:9">
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37">
+        <v>1075868</v>
+      </c>
+      <c r="H37">
+        <v>1108311</v>
+      </c>
+      <c r="I37">
+        <v>1411371</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G35">
-        <v>1075868</v>
-      </c>
-      <c r="H35">
-        <v>1108311</v>
-      </c>
-      <c r="I35">
-        <v>1411371</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="F37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39">
+      <c r="B41">
         <v>0.04</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>0.11</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>0.01</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="8">
-        <f>B39*$G$45/100</f>
+      <c r="F41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" s="8">
+        <f>B41*$G$47/100</f>
         <v>1922.0896</v>
       </c>
-      <c r="H39" s="8">
-        <f t="shared" ref="H39:I44" si="2">C39*$G$45/100</f>
+      <c r="H41" s="8">
+        <f t="shared" ref="H41:I46" si="2">C41*$G$47/100</f>
         <v>5285.7464</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I41" s="8">
         <f t="shared" si="2"/>
         <v>480.5224</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40">
+    <row r="42" spans="1:9">
+      <c r="A42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42">
         <v>21.23</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>22.71</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>94.64</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G40" s="8">
-        <f t="shared" ref="G40:G44" si="3">B40*$G$45/100</f>
+      <c r="F42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="8">
+        <f t="shared" ref="G42:G46" si="3">B42*$G$47/100</f>
         <v>1020149.0551999999</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H42" s="8">
         <f t="shared" si="2"/>
         <v>1091266.3704000001</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I42" s="8">
         <f t="shared" si="2"/>
         <v>4547663.9935999997</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41">
+    <row r="43" spans="1:9">
+      <c r="A43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43">
         <v>5.29</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>4.21</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>0.16</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="8">
+      <c r="F43" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43" s="8">
         <f t="shared" si="3"/>
         <v>254196.34960000002</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H43" s="8">
         <f t="shared" si="2"/>
         <v>202299.93039999998</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I43" s="8">
         <f t="shared" si="2"/>
         <v>7688.3584000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42">
+    <row r="44" spans="1:9">
+      <c r="A44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
         <v>1.24</v>
       </c>
-      <c r="C42">
+      <c r="C44">
         <v>1.23</v>
       </c>
-      <c r="D42">
+      <c r="D44">
         <v>3.58</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" s="8">
+      <c r="F44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G44" s="8">
         <f t="shared" si="3"/>
         <v>59584.777600000001</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H44" s="8">
         <f t="shared" si="2"/>
         <v>59104.255199999992</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I44" s="8">
         <f t="shared" si="2"/>
         <v>172027.01920000001</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43">
+    <row r="45" spans="1:9">
+      <c r="A45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45">
         <v>72.06</v>
       </c>
-      <c r="C43">
+      <c r="C45">
         <v>71.56</v>
       </c>
-      <c r="D43">
+      <c r="D45">
         <v>0.99</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G43" s="8">
+      <c r="F45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" s="8">
         <f t="shared" si="3"/>
         <v>3462644.4144000001</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H45" s="8">
         <f t="shared" si="2"/>
         <v>3438618.2944</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I45" s="8">
         <f t="shared" si="2"/>
         <v>47571.717599999996</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44">
+    <row r="46" spans="1:9">
+      <c r="A46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46">
         <v>0.3</v>
       </c>
-      <c r="C44">
+      <c r="C46">
         <v>0.32</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>0.8</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G44" s="8">
+      <c r="F46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="8">
         <f t="shared" si="3"/>
         <v>14415.671999999999</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H46" s="8">
         <f t="shared" si="2"/>
         <v>15376.7168</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I46" s="8">
         <f t="shared" si="2"/>
         <v>38441.792000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F45" t="s">
-        <v>73</v>
-      </c>
-      <c r="G45">
+    <row r="47" spans="1:9">
+      <c r="F47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47">
         <v>4805224</v>
       </c>
-      <c r="H45">
+      <c r="H47">
         <v>5359607</v>
       </c>
-      <c r="I45">
+      <c r="I47">
         <v>1454504</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECDB9F3-F29B-4465-8C62-E1D52B2C1777}">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{6C11D151-9560-5742-97A8-9C1B4498589C}">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>942</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2">
+        <v>132</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.14049600000000001</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2.69421</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2.8347060000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3">
+        <v>942</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3">
+        <v>133</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>3.3057900000000001E-2</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1.33884</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1.3718979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="11">
+        <v>134</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3">
+        <v>942</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="11">
+        <v>134</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="5">
+        <v>9.0743799999999997</v>
+      </c>
+      <c r="K7" s="5">
+        <v>17.4298</v>
+      </c>
+      <c r="L7" s="5">
+        <v>56.421500000000002</v>
+      </c>
+      <c r="M7" s="5">
+        <v>73.851299999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="16"/>
+      <c r="B8" s="11">
+        <v>135</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3">
+        <v>942</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="11">
+        <v>135</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="5">
+        <v>6.2479300000000002</v>
+      </c>
+      <c r="K8" s="5">
+        <v>6.2644599999999997</v>
+      </c>
+      <c r="L8" s="5">
+        <v>92.2727</v>
+      </c>
+      <c r="M8" s="5">
+        <v>98.53716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="3">
+        <v>941</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="11">
+        <v>136</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="5">
+        <v>5.1239699999999999</v>
+      </c>
+      <c r="K9" s="5">
+        <v>5.1405000000000003</v>
+      </c>
+      <c r="L9" s="5">
+        <v>93.933899999999994</v>
+      </c>
+      <c r="M9" s="5">
+        <v>99.074399999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="11">
+        <v>137</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3">
+        <v>941</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="11">
+        <v>137</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="5">
+        <v>75.7851</v>
+      </c>
+      <c r="K10" s="5">
+        <v>82.115700000000004</v>
+      </c>
+      <c r="L10" s="5">
+        <v>17.8843</v>
+      </c>
+      <c r="M10" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11">
+        <v>138</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="3">
+        <v>942</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="11">
+        <v>138</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11">
+        <v>88.603300000000004</v>
+      </c>
+      <c r="K11">
+        <v>88.628100000000003</v>
+      </c>
+      <c r="L11">
+        <v>11.3719</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="13"/>
+      <c r="B12" s="11">
+        <v>139</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3">
+        <v>941</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="11">
+        <v>139</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="5">
+        <v>98.305800000000005</v>
+      </c>
+      <c r="K12" s="5">
+        <v>98.421499999999995</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.5785100000000001</v>
+      </c>
+      <c r="M12" s="5">
+        <v>100.00001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="11">
+        <v>140</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="3">
+        <v>942</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="11">
+        <v>140</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="5">
+        <v>10.9339</v>
+      </c>
+      <c r="K16" s="5">
+        <v>21.578499999999998</v>
+      </c>
+      <c r="L16" s="5">
+        <v>20.619800000000001</v>
+      </c>
+      <c r="M16" s="5">
+        <v>42.198300000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="16"/>
+      <c r="B17" s="11">
+        <v>141</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3">
+        <v>942</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="11">
+        <v>141</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="5">
+        <v>11.504099999999999</v>
+      </c>
+      <c r="K17" s="5">
+        <v>11.545500000000001</v>
+      </c>
+      <c r="L17" s="5">
+        <v>16.776900000000001</v>
+      </c>
+      <c r="M17" s="5">
+        <v>28.322399999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="16"/>
+      <c r="B18" s="11">
+        <v>142</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3">
+        <v>941</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="11">
+        <v>142</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="5">
+        <v>12.6198</v>
+      </c>
+      <c r="K18" s="5">
+        <v>12.6777</v>
+      </c>
+      <c r="L18" s="5">
+        <v>8.30579</v>
+      </c>
+      <c r="M18" s="5">
+        <v>20.98349</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="11">
+        <v>143</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="3">
+        <v>942</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="11">
+        <v>143</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="5">
+        <v>75.264499999999998</v>
+      </c>
+      <c r="K19" s="5">
+        <v>81.843000000000004</v>
+      </c>
+      <c r="L19" s="5">
+        <v>18.157</v>
+      </c>
+      <c r="M19" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="13"/>
+      <c r="B20" s="11">
+        <v>144</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="3">
+        <v>942</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="11">
+        <v>144</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="5">
+        <v>88.950400000000002</v>
+      </c>
+      <c r="K20" s="5">
+        <v>88.966899999999995</v>
+      </c>
+      <c r="L20" s="5">
+        <v>11.033099999999999</v>
+      </c>
+      <c r="M20" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="13"/>
+      <c r="B21" s="11">
+        <v>145</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3">
+        <v>941</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="11">
+        <v>145</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="5">
+        <v>98.479299999999995</v>
+      </c>
+      <c r="K21" s="5">
+        <v>98.553700000000006</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1.44628</v>
+      </c>
+      <c r="M21" s="5">
+        <v>99.999979999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="2" customFormat="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="11">
+        <v>146</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="3">
+        <v>942</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="11">
+        <v>146</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="5">
+        <v>9.7438000000000002</v>
+      </c>
+      <c r="K25" s="5">
+        <v>18.867799999999999</v>
+      </c>
+      <c r="L25" s="5">
+        <v>36.7438</v>
+      </c>
+      <c r="M25" s="5">
+        <v>55.611600000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="16"/>
+      <c r="B26" s="11">
+        <v>147</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="3">
+        <v>942</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="11">
+        <v>147</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="5">
+        <v>6.19008</v>
+      </c>
+      <c r="K26" s="5">
+        <v>6.2479300000000002</v>
+      </c>
+      <c r="L26" s="5">
+        <v>91.289299999999997</v>
+      </c>
+      <c r="M26" s="5">
+        <v>97.537229999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="16"/>
+      <c r="B27" s="11">
+        <v>148</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="3">
+        <v>941</v>
+      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="11">
+        <v>148</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" s="5">
+        <v>5.09917</v>
+      </c>
+      <c r="K27" s="5">
+        <v>5.1074400000000004</v>
+      </c>
+      <c r="L27" s="5">
+        <v>93.7851</v>
+      </c>
+      <c r="M27" s="5">
+        <v>98.892539999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="11">
+        <v>149</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3">
+        <v>941</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" s="11">
+        <v>149</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="5">
+        <v>75.107399999999998</v>
+      </c>
+      <c r="K28" s="5">
+        <v>81.876000000000005</v>
+      </c>
+      <c r="L28" s="5">
+        <v>18.123999999999999</v>
+      </c>
+      <c r="M28" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="13"/>
+      <c r="B29" s="11">
+        <v>150</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="3">
+        <v>942</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="11">
+        <v>150</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="5">
+        <v>88.603300000000004</v>
+      </c>
+      <c r="K29" s="5">
+        <v>88.611599999999996</v>
+      </c>
+      <c r="L29" s="5">
+        <v>11.388400000000001</v>
+      </c>
+      <c r="M29" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="13"/>
+      <c r="B30" s="11">
+        <v>151</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="3">
+        <v>941</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="11">
+        <v>151</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="5">
+        <v>98.586799999999997</v>
+      </c>
+      <c r="K30" s="5">
+        <v>98.603300000000004</v>
+      </c>
+      <c r="L30" s="5">
+        <v>1.39669</v>
+      </c>
+      <c r="M30" s="5">
+        <v>99.999989999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A25:A27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the performance spreadsheet
modified:   cpu_network_performance.xlsx
</commit_message>
<xml_diff>
--- a/data/cpu_network_performance.xlsx
+++ b/data/cpu_network_performance.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binghamton0-my.sharepoint.com/personal/tcheng8_binghamton_edu/Documents/itri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="29D64C58418C33B10946EF46E32E0DF452F98909" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{802C109F-8405-4982-A8CA-2DB5EB8FB8A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3B49874-806C-40BD-A64F-ACA06518EA65}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="25960" windowHeight="14700" tabRatio="993" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="460" windowWidth="25960" windowHeight="14700" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
     <sheet name="atop_1p26_2010" sheetId="4" r:id="rId2"/>
     <sheet name="atop_2p3p0_2017" sheetId="6" r:id="rId3"/>
-    <sheet name="poll_halt_ns" sheetId="7" r:id="rId4"/>
+    <sheet name="halt_poll_ns" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171026" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="89">
   <si>
     <t>experiment</t>
   </si>
@@ -293,6 +293,15 @@
   <si>
     <t>halt_poll_ns=200000</t>
   </si>
+  <si>
+    <t>IDLE=HLT, 154 - 156</t>
+  </si>
+  <si>
+    <t>IDLE=POLL, 157- 159</t>
+  </si>
+  <si>
+    <t>EXCEPTION_NMI</t>
+  </si>
 </sst>
 </file>
 
@@ -384,6 +393,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,15 +408,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2997,10 +3006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView topLeftCell="A125" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -5186,6 +5195,142 @@
       </c>
       <c r="E137" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139">
+        <v>152</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" t="s">
+        <v>54</v>
+      </c>
+      <c r="D139" t="s">
+        <v>43</v>
+      </c>
+      <c r="E139" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140">
+        <v>153</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" t="s">
+        <v>54</v>
+      </c>
+      <c r="D140" t="s">
+        <v>44</v>
+      </c>
+      <c r="E140" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142">
+        <v>154</v>
+      </c>
+      <c r="B142" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" t="s">
+        <v>54</v>
+      </c>
+      <c r="D142" t="s">
+        <v>42</v>
+      </c>
+      <c r="E142" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143">
+        <v>155</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" t="s">
+        <v>54</v>
+      </c>
+      <c r="D143" t="s">
+        <v>43</v>
+      </c>
+      <c r="E143" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144">
+        <v>156</v>
+      </c>
+      <c r="B144" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144" t="s">
+        <v>54</v>
+      </c>
+      <c r="D144" t="s">
+        <v>44</v>
+      </c>
+      <c r="E144" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145">
+        <v>157</v>
+      </c>
+      <c r="B145" t="s">
+        <v>9</v>
+      </c>
+      <c r="C145" t="s">
+        <v>54</v>
+      </c>
+      <c r="D145" t="s">
+        <v>45</v>
+      </c>
+      <c r="E145" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146">
+        <v>158</v>
+      </c>
+      <c r="B146" t="s">
+        <v>9</v>
+      </c>
+      <c r="C146" t="s">
+        <v>54</v>
+      </c>
+      <c r="D146" t="s">
+        <v>46</v>
+      </c>
+      <c r="E146" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147">
+        <v>159</v>
+      </c>
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" t="s">
+        <v>54</v>
+      </c>
+      <c r="D147" t="s">
+        <v>47</v>
+      </c>
+      <c r="E147" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -5238,19 +5383,19 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1"/>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="14" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="11">
@@ -5286,7 +5431,7 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="16"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="11">
         <v>102</v>
       </c>
@@ -5321,7 +5466,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="11">
         <v>104</v>
       </c>
@@ -5357,7 +5502,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="11">
@@ -5395,7 +5540,7 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="11">
         <v>108</v>
       </c>
@@ -5407,7 +5552,7 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="11">
         <v>110</v>
       </c>
@@ -5439,7 +5584,7 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="11">
@@ -5462,7 +5607,7 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="11">
         <v>102</v>
       </c>
@@ -5483,7 +5628,7 @@
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="11">
         <v>104</v>
       </c>
@@ -5504,7 +5649,7 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="11">
@@ -5527,7 +5672,7 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="11">
         <v>108</v>
       </c>
@@ -5548,7 +5693,7 @@
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="11">
         <v>110</v>
       </c>
@@ -6091,8 +6236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="A28" sqref="A28:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -6123,19 +6268,19 @@
         <v>69</v>
       </c>
       <c r="G1" s="3"/>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="14" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="11">
@@ -6172,7 +6317,7 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="16"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="11">
         <v>114</v>
       </c>
@@ -6210,7 +6355,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="11">
         <v>116</v>
       </c>
@@ -6246,7 +6391,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="11">
@@ -6284,7 +6429,7 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="11">
         <v>120</v>
       </c>
@@ -6299,7 +6444,7 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="11">
         <v>122</v>
       </c>
@@ -6344,7 +6489,7 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="11">
@@ -6370,7 +6515,7 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="11">
         <v>114</v>
       </c>
@@ -6391,7 +6536,7 @@
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="11">
         <v>116</v>
       </c>
@@ -6412,7 +6557,7 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="11">
@@ -6435,7 +6580,7 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="11">
         <v>120</v>
       </c>
@@ -6456,7 +6601,7 @@
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="11">
         <v>122</v>
       </c>
@@ -6507,7 +6652,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="3">
@@ -6530,7 +6675,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="16"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="11">
         <v>124</v>
       </c>
@@ -6551,7 +6696,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="16"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="11">
         <v>125</v>
       </c>
@@ -6572,7 +6717,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="16"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="11">
         <v>126</v>
       </c>
@@ -6593,7 +6738,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="11">
@@ -6616,7 +6761,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="11">
         <v>127</v>
       </c>
@@ -6637,7 +6782,7 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="11">
         <v>128</v>
       </c>
@@ -6658,7 +6803,7 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="11">
         <v>129</v>
       </c>
@@ -7192,18 +7337,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECDB9F3-F29B-4465-8C62-E1D52B2C1777}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{6C11D151-9560-5742-97A8-9C1B4498589C}">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0" xr3:uid="{6C11D151-9560-5742-97A8-9C1B4498589C}">
+      <selection activeCell="H52" sqref="H52:J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7240,7 +7385,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B2">
@@ -7252,7 +7397,7 @@
       <c r="D2">
         <v>942</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="14" t="s">
         <v>58</v>
       </c>
       <c r="H2">
@@ -7272,7 +7417,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B3">
@@ -7284,7 +7429,7 @@
       <c r="D3">
         <v>942</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="15" t="s">
         <v>59</v>
       </c>
       <c r="H3">
@@ -7339,7 +7484,7 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="11">
@@ -7351,7 +7496,7 @@
       <c r="D7" s="3">
         <v>942</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="19" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="11">
@@ -7374,7 +7519,7 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="11">
         <v>135</v>
       </c>
@@ -7384,7 +7529,7 @@
       <c r="D8" s="3">
         <v>942</v>
       </c>
-      <c r="G8" s="16"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="11">
         <v>135</v>
       </c>
@@ -7405,7 +7550,7 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="11">
         <v>136</v>
       </c>
@@ -7415,7 +7560,7 @@
       <c r="D9" s="3">
         <v>941</v>
       </c>
-      <c r="G9" s="16"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="11">
         <v>136</v>
       </c>
@@ -7436,7 +7581,7 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="11">
@@ -7448,7 +7593,7 @@
       <c r="D10" s="3">
         <v>941</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="16" t="s">
         <v>59</v>
       </c>
       <c r="H10" s="11">
@@ -7471,7 +7616,7 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="13"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="11">
         <v>138</v>
       </c>
@@ -7481,7 +7626,7 @@
       <c r="D11" s="3">
         <v>942</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="11">
         <v>138</v>
       </c>
@@ -7502,7 +7647,7 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="13"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="11">
         <v>139</v>
       </c>
@@ -7512,7 +7657,7 @@
       <c r="D12" s="3">
         <v>941</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="11">
         <v>139</v>
       </c>
@@ -7583,7 +7728,7 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B16" s="11">
@@ -7595,7 +7740,7 @@
       <c r="D16" s="3">
         <v>942</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="19" t="s">
         <v>58</v>
       </c>
       <c r="H16" s="11">
@@ -7618,7 +7763,7 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="16"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="11">
         <v>141</v>
       </c>
@@ -7628,7 +7773,7 @@
       <c r="D17" s="3">
         <v>942</v>
       </c>
-      <c r="G17" s="16"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="11">
         <v>141</v>
       </c>
@@ -7649,7 +7794,7 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="16"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="11">
         <v>142</v>
       </c>
@@ -7659,7 +7804,7 @@
       <c r="D18" s="3">
         <v>941</v>
       </c>
-      <c r="G18" s="16"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="11">
         <v>142</v>
       </c>
@@ -7680,7 +7825,7 @@
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="11">
@@ -7692,7 +7837,7 @@
       <c r="D19" s="3">
         <v>942</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="16" t="s">
         <v>59</v>
       </c>
       <c r="H19" s="11">
@@ -7715,7 +7860,7 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="11">
         <v>144</v>
       </c>
@@ -7725,7 +7870,7 @@
       <c r="D20" s="3">
         <v>942</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="11">
         <v>144</v>
       </c>
@@ -7746,7 +7891,7 @@
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="11">
         <v>145</v>
       </c>
@@ -7756,7 +7901,7 @@
       <c r="D21" s="3">
         <v>941</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="11">
         <v>145</v>
       </c>
@@ -7784,10 +7929,10 @@
       <c r="G22" s="12"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
@@ -7825,7 +7970,7 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="11">
@@ -7837,7 +7982,7 @@
       <c r="D25" s="3">
         <v>942</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="19" t="s">
         <v>58</v>
       </c>
       <c r="H25" s="11">
@@ -7860,7 +8005,7 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="16"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="11">
         <v>147</v>
       </c>
@@ -7870,7 +8015,7 @@
       <c r="D26" s="3">
         <v>942</v>
       </c>
-      <c r="G26" s="16"/>
+      <c r="G26" s="19"/>
       <c r="H26" s="11">
         <v>147</v>
       </c>
@@ -7891,7 +8036,7 @@
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="16"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="11">
         <v>148</v>
       </c>
@@ -7901,7 +8046,7 @@
       <c r="D27" s="3">
         <v>941</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="11">
         <v>148</v>
       </c>
@@ -7922,7 +8067,7 @@
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="11">
@@ -7934,7 +8079,7 @@
       <c r="D28" s="3">
         <v>941</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="16" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="11">
@@ -7957,7 +8102,7 @@
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="11">
         <v>150</v>
       </c>
@@ -7967,7 +8112,7 @@
       <c r="D29" s="3">
         <v>942</v>
       </c>
-      <c r="G29" s="13"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="11">
         <v>150</v>
       </c>
@@ -7988,7 +8133,7 @@
       </c>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="11">
         <v>151</v>
       </c>
@@ -7998,7 +8143,7 @@
       <c r="D30" s="3">
         <v>941</v>
       </c>
-      <c r="G30" s="13"/>
+      <c r="G30" s="16"/>
       <c r="H30" s="11">
         <v>151</v>
       </c>
@@ -8018,20 +8163,664 @@
         <v>99.999989999999997</v>
       </c>
     </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="11">
+        <v>152</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="3">
+        <v>942</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="11">
+        <v>152</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J34" s="5">
+        <v>10.8264</v>
+      </c>
+      <c r="K34" s="5">
+        <v>10.9008</v>
+      </c>
+      <c r="L34" s="5">
+        <v>14.6281</v>
+      </c>
+      <c r="M34" s="5">
+        <v>25.5289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="19"/>
+      <c r="B35" s="11">
+        <v>153</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="3">
+        <v>941</v>
+      </c>
+      <c r="G35" s="19"/>
+      <c r="H35" s="11">
+        <v>153</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" s="5">
+        <v>12.867800000000001</v>
+      </c>
+      <c r="K35" s="5">
+        <v>12.9008</v>
+      </c>
+      <c r="L35" s="5">
+        <v>8</v>
+      </c>
+      <c r="M35" s="5">
+        <v>20.9008</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="G38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40">
+        <v>0.01</v>
+      </c>
+      <c r="C40">
+        <v>0.02</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="8">
+        <f>B40*$H$48/100</f>
+        <v>109.1161</v>
+      </c>
+      <c r="I40" s="8">
+        <f t="shared" ref="I40:J47" si="0">C40*$H$48/100</f>
+        <v>218.23220000000001</v>
+      </c>
+      <c r="J40" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C41">
+        <v>0.02</v>
+      </c>
+      <c r="D41">
+        <v>0.05</v>
+      </c>
+      <c r="G41" t="s">
+        <v>73</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" ref="H41:H47" si="1">B41*$H$48/100</f>
+        <v>1527.6254000000001</v>
+      </c>
+      <c r="I41" s="8">
+        <f t="shared" si="0"/>
+        <v>218.23220000000001</v>
+      </c>
+      <c r="J41" s="8">
+        <f t="shared" si="0"/>
+        <v>545.58050000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42">
+        <v>7.53</v>
+      </c>
+      <c r="C42">
+        <v>9.52</v>
+      </c>
+      <c r="D42">
+        <v>9.11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" s="8">
+        <f t="shared" si="1"/>
+        <v>82164.423299999995</v>
+      </c>
+      <c r="I42" s="8">
+        <f t="shared" si="0"/>
+        <v>103878.52719999998</v>
+      </c>
+      <c r="J42" s="8">
+        <f t="shared" si="0"/>
+        <v>99404.767099999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>69.61</v>
+      </c>
+      <c r="C43">
+        <v>63.06</v>
+      </c>
+      <c r="D43">
+        <v>85.71</v>
+      </c>
+      <c r="G43" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="8">
+        <f t="shared" si="1"/>
+        <v>759557.17209999997</v>
+      </c>
+      <c r="I43" s="8">
+        <f t="shared" si="0"/>
+        <v>688086.12659999996</v>
+      </c>
+      <c r="J43" s="8">
+        <f t="shared" si="0"/>
+        <v>935234.09309999982</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
+        <v>17.29</v>
+      </c>
+      <c r="C44">
+        <v>21.48</v>
+      </c>
+      <c r="D44">
+        <v>0.2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="1"/>
+        <v>188661.73689999999</v>
+      </c>
+      <c r="I44" s="8">
+        <f t="shared" si="0"/>
+        <v>234381.38280000002</v>
+      </c>
+      <c r="J44" s="8">
+        <f t="shared" si="0"/>
+        <v>2182.3220000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45">
+        <v>5.3</v>
+      </c>
+      <c r="C45">
+        <v>5.62</v>
+      </c>
+      <c r="D45">
+        <v>4.59</v>
+      </c>
+      <c r="G45" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="1"/>
+        <v>57831.532999999996</v>
+      </c>
+      <c r="I45" s="8">
+        <f t="shared" si="0"/>
+        <v>61323.248200000002</v>
+      </c>
+      <c r="J45" s="8">
+        <f t="shared" si="0"/>
+        <v>50084.289900000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46">
+        <v>0.02</v>
+      </c>
+      <c r="C46">
+        <v>0.04</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="1"/>
+        <v>218.23220000000001</v>
+      </c>
+      <c r="I46" s="8">
+        <f t="shared" si="0"/>
+        <v>436.46440000000001</v>
+      </c>
+      <c r="J46" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47">
+        <v>0.18</v>
+      </c>
+      <c r="C47">
+        <v>0.3</v>
+      </c>
+      <c r="D47">
+        <v>0.16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H47" s="8">
+        <f t="shared" si="1"/>
+        <v>1964.0897999999997</v>
+      </c>
+      <c r="I47" s="8">
+        <f t="shared" si="0"/>
+        <v>3273.4829999999997</v>
+      </c>
+      <c r="J47" s="8">
+        <f t="shared" si="0"/>
+        <v>1745.8576</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="H48">
+        <v>1091161</v>
+      </c>
+      <c r="I48">
+        <v>1040794</v>
+      </c>
+      <c r="J48">
+        <v>1331658</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="G50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0.05</v>
+      </c>
+      <c r="G52" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" s="9">
+        <f>B52*$H$59/100</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="9">
+        <f t="shared" ref="I52:J58" si="2">C52*$H$59/100</f>
+        <v>0</v>
+      </c>
+      <c r="J52" s="9">
+        <f t="shared" si="2"/>
+        <v>2429.1190000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0.01</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" s="9">
+        <f t="shared" ref="H53:H58" si="3">B53*$H$59/100</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="9">
+        <f t="shared" si="2"/>
+        <v>485.82379999999995</v>
+      </c>
+      <c r="J53" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54">
+        <v>29.27</v>
+      </c>
+      <c r="C54">
+        <v>22.39</v>
+      </c>
+      <c r="D54">
+        <v>95.02</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H54" s="9">
+        <f t="shared" si="3"/>
+        <v>1422006.2626</v>
+      </c>
+      <c r="I54" s="9">
+        <f t="shared" si="2"/>
+        <v>1087759.4882</v>
+      </c>
+      <c r="J54" s="9">
+        <f t="shared" si="2"/>
+        <v>4616297.7476000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C55">
+        <v>4.3</v>
+      </c>
+      <c r="D55">
+        <v>0.08</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H55" s="9">
+        <f t="shared" si="3"/>
+        <v>247770.13799999998</v>
+      </c>
+      <c r="I55" s="9">
+        <f t="shared" si="2"/>
+        <v>208904.234</v>
+      </c>
+      <c r="J55" s="9">
+        <f t="shared" si="2"/>
+        <v>3886.5903999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C56">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D56">
+        <v>3.35</v>
+      </c>
+      <c r="G56" t="s">
+        <v>77</v>
+      </c>
+      <c r="H56" s="9">
+        <f t="shared" si="3"/>
+        <v>53926.441800000008</v>
+      </c>
+      <c r="I56" s="9">
+        <f t="shared" si="2"/>
+        <v>54898.089399999997</v>
+      </c>
+      <c r="J56" s="9">
+        <f t="shared" si="2"/>
+        <v>162750.973</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57">
+        <v>64.39</v>
+      </c>
+      <c r="C57">
+        <v>71.959999999999994</v>
+      </c>
+      <c r="D57">
+        <v>0.95</v>
+      </c>
+      <c r="G57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H57" s="9">
+        <f t="shared" si="3"/>
+        <v>3128219.4482</v>
+      </c>
+      <c r="I57" s="9">
+        <f t="shared" si="2"/>
+        <v>3495988.0647999998</v>
+      </c>
+      <c r="J57" s="9">
+        <f t="shared" si="2"/>
+        <v>46153.260999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58">
+        <v>0.34</v>
+      </c>
+      <c r="C58">
+        <v>0.34</v>
+      </c>
+      <c r="D58">
+        <v>0.71</v>
+      </c>
+      <c r="G58" t="s">
+        <v>79</v>
+      </c>
+      <c r="H58" s="9">
+        <f t="shared" si="3"/>
+        <v>16518.0092</v>
+      </c>
+      <c r="I58" s="9">
+        <f t="shared" si="2"/>
+        <v>16518.0092</v>
+      </c>
+      <c r="J58" s="9">
+        <f t="shared" si="2"/>
+        <v>34493.489800000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="H59">
+        <v>4858238</v>
+      </c>
+      <c r="I59">
+        <v>5408409</v>
+      </c>
+      <c r="J59">
+        <v>1451642</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="G28:G30"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="G19:G21"/>
     <mergeCell ref="G25:G27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update the performance spread sheet
modified:   cpu_network_performance.xlsx
</commit_message>
<xml_diff>
--- a/data/cpu_network_performance.xlsx
+++ b/data/cpu_network_performance.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binghamton0-my.sharepoint.com/personal/tcheng8_binghamton_edu/Documents/itri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3B49874-806C-40BD-A64F-ACA06518EA65}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="BC86BABE7FB80D48AF90F663CDB92E6A9514898B" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="25960" windowHeight="14700" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="10980" tabRatio="993" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="experiments" sheetId="1" r:id="rId1"/>
     <sheet name="atop_1p26_2010" sheetId="4" r:id="rId2"/>
     <sheet name="atop_2p3p0_2017" sheetId="6" r:id="rId3"/>
     <sheet name="halt_poll_ns" sheetId="7" r:id="rId4"/>
+    <sheet name="halt_poll_ns_cpu_util_brkdwn" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171026" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="97">
   <si>
     <t>experiment</t>
   </si>
@@ -302,6 +303,30 @@
   <si>
     <t>EXCEPTION_NMI</t>
   </si>
+  <si>
+    <t>usr</t>
+  </si>
+  <si>
+    <t>nice</t>
+  </si>
+  <si>
+    <t>sys</t>
+  </si>
+  <si>
+    <t>irq</t>
+  </si>
+  <si>
+    <t>softirq</t>
+  </si>
+  <si>
+    <t>steal</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>idle</t>
+  </si>
 </sst>
 </file>
 
@@ -375,7 +400,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -407,6 +432,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1537,6 +1565,1383 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPU</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Utilization</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>IDLE=HLT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>baremetal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$2:$L$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.14049600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.983471</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71074400000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6528999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97.148759999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5310-4C89-8692-C4BE816EE72B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>virtio-net</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21.578512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.132231000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>2.487603</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>10.933884000000001</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.4792999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>57.694215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5310-4C89-8692-C4BE816EE72B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vhost-net</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.545455</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.380165</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.3966940000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>11.504132</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.1321999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>71.371900999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5310-4C89-8692-C4BE816EE72B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vfio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$1:$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$5:$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12.677686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3057850000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>12.619835</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.9586999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>79.016529000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5310-4C89-8692-C4BE816EE72B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="518546992"/>
+        <c:axId val="518546576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="518546992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518546576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="518546576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518546992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CPU Utilization</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IDLE=POLL</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>baremetal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$8:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.3057999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.033058</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30578499999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6528999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>98.61157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5889-4944-ACA1-9D3F215F826C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>virtio-net</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$8:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>81.842974999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.834711</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3223140000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.264463000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5889-4944-ACA1-9D3F215F826C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vhost-net</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$8:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$11:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>88.966942000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2644630000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7685950000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.950412999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5889-4944-ACA1-9D3F215F826C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>vfio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$8:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>usr</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nice</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sys</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>irq</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>softirq</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>steal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>guest</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>wait</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>halt_poll_ns_cpu_util_brkdwn!$D$12:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>98.553719000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4462809999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.479338999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5889-4944-ACA1-9D3F215F826C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="533653136"/>
+        <c:axId val="533652304"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="533653136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533652304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533652304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533653136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1578,6 +2983,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2623,6 +4108,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2701,6 +5192,87 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3012,7 +5584,7 @@
       <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
@@ -5351,7 +7923,7 @@
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.625" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="17.625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="23.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
@@ -6236,11 +8808,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="A28" sqref="A28:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
@@ -7336,11 +9908,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECDB9F3-F29B-4465-8C62-E1D52B2C1777}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0" xr3:uid="{6C11D151-9560-5742-97A8-9C1B4498589C}">
-      <selection activeCell="H52" sqref="H52:J58"/>
+    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+      <selection activeCell="G15" sqref="G15:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -8824,4 +11396,698 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:V16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+      <selection activeCell="X11" sqref="X11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3">
+        <v>132</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.14049600000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.983471</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.71074400000000004</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1.6528999999999999E-2</v>
+      </c>
+      <c r="L2">
+        <v>97.148759999999996</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="19"/>
+      <c r="B3" s="11">
+        <v>140</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="5">
+        <v>21.578512</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>18.132231000000001</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2.487603</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>10.933884000000001</v>
+      </c>
+      <c r="K3">
+        <v>2.4792999999999999E-2</v>
+      </c>
+      <c r="L3">
+        <v>57.694215</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0.14049600000000001</v>
+      </c>
+      <c r="P3" s="5">
+        <v>21.578512</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>11.545455</v>
+      </c>
+      <c r="R3" s="5">
+        <v>12.677686</v>
+      </c>
+      <c r="S3">
+        <v>3.3057999999999997E-2</v>
+      </c>
+      <c r="T3">
+        <v>81.842974999999996</v>
+      </c>
+      <c r="U3">
+        <v>88.966942000000003</v>
+      </c>
+      <c r="V3">
+        <v>98.553719000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="19"/>
+      <c r="B4" s="11">
+        <v>141</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="5">
+        <v>11.545455</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>13.380165</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>3.3966940000000001</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>11.504132</v>
+      </c>
+      <c r="K4">
+        <v>4.1321999999999998E-2</v>
+      </c>
+      <c r="L4">
+        <v>71.371900999999994</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="19"/>
+      <c r="B5" s="11">
+        <v>142</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="5">
+        <v>12.677686</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>8.3057850000000002</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>12.619835</v>
+      </c>
+      <c r="K5">
+        <v>4.9586999999999999E-2</v>
+      </c>
+      <c r="L5">
+        <v>79.016529000000006</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1.983471</v>
+      </c>
+      <c r="P5" s="5">
+        <v>18.132231000000001</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>13.380165</v>
+      </c>
+      <c r="R5" s="5">
+        <v>8.3057850000000002</v>
+      </c>
+      <c r="S5">
+        <v>1.033058</v>
+      </c>
+      <c r="T5">
+        <v>11.834711</v>
+      </c>
+      <c r="U5">
+        <v>6.2644630000000001</v>
+      </c>
+      <c r="V5">
+        <v>1.4462809999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="N6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="N7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7">
+        <v>0.71074400000000004</v>
+      </c>
+      <c r="P7">
+        <v>2.487603</v>
+      </c>
+      <c r="Q7">
+        <v>3.3966940000000001</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0.30578499999999997</v>
+      </c>
+      <c r="T7">
+        <v>6.3223140000000004</v>
+      </c>
+      <c r="U7">
+        <v>4.7685950000000004</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9">
+        <v>3.3057999999999997E-2</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.033058</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.30578499999999997</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1.6528999999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>98.61157</v>
+      </c>
+      <c r="N9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>10.933884000000001</v>
+      </c>
+      <c r="Q9">
+        <v>11.504132</v>
+      </c>
+      <c r="R9">
+        <v>12.619835</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>75.264463000000006</v>
+      </c>
+      <c r="U9">
+        <v>88.950412999999998</v>
+      </c>
+      <c r="V9">
+        <v>98.479338999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="16"/>
+      <c r="B10" s="11">
+        <v>143</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>81.842974999999996</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>11.834711</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>6.3223140000000004</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>75.264463000000006</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10">
+        <v>1.6528999999999999E-2</v>
+      </c>
+      <c r="P10">
+        <v>2.4792999999999999E-2</v>
+      </c>
+      <c r="Q10">
+        <v>4.1321999999999998E-2</v>
+      </c>
+      <c r="R10">
+        <v>4.9586999999999999E-2</v>
+      </c>
+      <c r="S10">
+        <v>1.6528999999999999E-2</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11">
+        <v>144</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>88.966942000000003</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>6.2644630000000001</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>4.7685950000000004</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>88.950412999999998</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11">
+        <v>97.148759999999996</v>
+      </c>
+      <c r="P11">
+        <v>57.694215</v>
+      </c>
+      <c r="Q11">
+        <v>71.371900999999994</v>
+      </c>
+      <c r="R11">
+        <v>79.016529000000006</v>
+      </c>
+      <c r="S11">
+        <v>98.61157</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="16"/>
+      <c r="B12" s="11">
+        <v>145</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>98.553719000000001</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1.4462809999999999</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>98.479338999999996</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A9:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>